<commit_message>
Updated ZAF model - 2025-07-29 14:21
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_ZAF/ReportDefs_vervestacks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D3B86D-5E44-469A-9BFD-27A22346152F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5F907D-7621-4CB6-B08A-0C1946E57417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
   <si>
     <t>Unit</t>
   </si>
@@ -506,6 +506,12 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Trd*</t>
+  </si>
+  <si>
+    <t>Trade</t>
   </si>
 </sst>
 </file>
@@ -1645,7 +1651,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A8EC7F-95E3-4526-8B78-C58A96098159}">
   <dimension ref="C1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -1875,10 +1881,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADB714-E6AA-4E3E-B77B-62B65BA0E218}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2155,6 +2161,17 @@
       </c>
       <c r="C22" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ZAF model - 2025-07-31 23:49
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/ReportDefs_vervestacks.xlsx
+++ b/VerveStacks_ZAF/ReportDefs_vervestacks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5F907D-7621-4CB6-B08A-0C1946E57417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AD581D-C637-43E8-9A19-5097D8EA4F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenMap" sheetId="56" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="145">
   <si>
     <t>Unit</t>
   </si>
@@ -115,9 +115,6 @@
     <t>TS</t>
   </si>
   <si>
-    <t>ELC</t>
-  </si>
-  <si>
     <t>VAR_CAP</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
     <t>c_neg_andor</t>
   </si>
   <si>
-    <t>ELE,STG</t>
-  </si>
-  <si>
     <t>Elec New Capacity</t>
   </si>
   <si>
@@ -472,9 +466,6 @@
     <t>Wind</t>
   </si>
   <si>
-    <t>-ElcAgg*</t>
-  </si>
-  <si>
     <t>p,t</t>
   </si>
   <si>
@@ -512,6 +503,18 @@
   </si>
   <si>
     <t>Trade</t>
+  </si>
+  <si>
+    <t>ELE,STG,IRE</t>
+  </si>
+  <si>
+    <t>ELE,IRE</t>
+  </si>
+  <si>
+    <t>-ElcAgg*,-*EV*</t>
+  </si>
+  <si>
+    <t>ELC,ELC_???-???</t>
   </si>
 </sst>
 </file>
@@ -1075,55 +1078,55 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="B1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M1" t="s">
         <v>8</v>
       </c>
       <c r="N1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:15">
       <c r="I2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" t="s">
         <v>49</v>
-      </c>
-      <c r="L2" t="s">
-        <v>50</v>
       </c>
       <c r="M2" t="s">
         <v>6</v>
       </c>
       <c r="N2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" t="s">
         <v>86</v>
-      </c>
-      <c r="H4" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1132,10 +1135,10 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" t="str">
         <f>"sg_"&amp;I2</f>
@@ -1180,7 +1183,7 @@
         <v>Fixed</v>
       </c>
       <c r="I6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O6">
         <v>1</v>
@@ -1208,7 +1211,7 @@
         <v>V1G</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="O7">
         <v>2</v>
@@ -1236,7 +1239,7 @@
         <v>V2G</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O8">
         <v>3</v>
@@ -1262,18 +1265,18 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1282,10 +1285,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
         <v>56</v>
-      </c>
-      <c r="G2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1320,32 +1323,32 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <f>1/8.76</f>
@@ -1354,13 +1357,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4">
         <f>1/8.76*100</f>
@@ -1377,9 +1380,9 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -1410,39 +1413,39 @@
   <sheetData>
     <row r="1" spans="1:21" ht="17.25" thickBot="1">
       <c r="A1" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="15" thickTop="1" thickBot="1">
       <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>22</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>0</v>
@@ -1451,7 +1454,7 @@
         <v>10</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" s="6" t="s">
         <v>2</v>
@@ -1460,56 +1463,62 @@
         <v>1</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Q2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>76</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:21">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
       <c r="N3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="P3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="Q3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:21">
       <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N4" t="s">
+        <v>102</v>
+      </c>
+      <c r="P4" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="K4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" t="s">
-        <v>104</v>
-      </c>
-      <c r="P4" t="s">
-        <v>46</v>
-      </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T4" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U4" s="8"/>
     </row>
@@ -1517,125 +1526,134 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>142</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>144</v>
       </c>
       <c r="K5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="P5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" t="s">
+        <v>57</v>
+      </c>
+      <c r="P6" t="s">
         <v>78</v>
       </c>
-      <c r="C6" t="s">
-        <v>103</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K6" t="s">
-        <v>111</v>
-      </c>
-      <c r="N6" t="s">
-        <v>58</v>
-      </c>
-      <c r="P6" t="s">
-        <v>79</v>
-      </c>
       <c r="Q6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K7" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7" t="s">
         <v>38</v>
-      </c>
-      <c r="K7" t="s">
-        <v>59</v>
-      </c>
-      <c r="N7" t="s">
-        <v>107</v>
-      </c>
-      <c r="P7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" t="s">
         <v>62</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>63</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" t="s">
+        <v>107</v>
+      </c>
+      <c r="N9" t="s">
         <v>65</v>
       </c>
-      <c r="K9" t="s">
-        <v>109</v>
-      </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q9" t="s">
         <v>66</v>
-      </c>
-      <c r="P9" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="N10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1670,15 +1688,15 @@
   <sheetData>
     <row r="1" spans="3:11">
       <c r="C1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="3:11">
       <c r="C2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>2</v>
@@ -1687,42 +1705,42 @@
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="3:11">
       <c r="C3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1750,18 +1768,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1785,18 +1803,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1824,18 +1842,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1860,18 +1878,18 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
-      </c>
-      <c r="C2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1883,7 +1901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10ADB714-E6AA-4E3E-B77B-62B65BA0E218}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -1899,71 +1917,71 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s">
         <v>89</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>90</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>91</v>
-      </c>
-      <c r="G2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C3" t="str">
         <f>D3</f>
         <v>CCGT</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ref="C4:C20" si="0">D4</f>
         <v>Int Comb</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>Gas_Oil Steam</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1975,67 +1993,67 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>OCGT (Peaker)</v>
       </c>
       <c r="D7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>Subcritical Coal</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>Supercritical Coal</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>IGCC</v>
       </c>
       <c r="D10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Bioenergy</v>
       </c>
       <c r="D11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2047,43 +2065,43 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Wind onshore</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>Wind offshore</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Geothermal</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
@@ -2095,7 +2113,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2107,46 +2125,46 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
         <v>Hydro pumped stg</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>Util Batt Stg</v>
       </c>
       <c r="D19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>EV Batt</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C21" t="s">
         <v>5</v>
@@ -2154,24 +2172,24 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C23" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2199,33 +2217,33 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
         <v>98</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>99</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>101</v>
-      </c>
-      <c r="G2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H2" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>